<commit_message>
Added test cases for Home
</commit_message>
<xml_diff>
--- a/src/test/java/com/seopa/tests/automated/test/cases/CarRegistrationLookUp01.xlsx
+++ b/src/test/java/com/seopa/tests/automated/test/cases/CarRegistrationLookUp01.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="72">
   <si>
     <t>Element Type</t>
   </si>
@@ -303,12 +303,55 @@
   <si>
     <t>//input[@name="vehicle_side" and @value="Y"]</t>
   </si>
+  <si>
+    <t>fake_vehicle_confirm</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color indexed="16"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>vehicle_registration_number</t>
+    </r>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>EXI5697</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color indexed="16"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>find_button</t>
+    </r>
+  </si>
+  <si>
+    <t>linktext</t>
+  </si>
+  <si>
+    <t>Find</t>
+  </si>
+  <si>
+    <t>//input[@name="registration_number_question" and @value="Y"]</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -340,6 +383,12 @@
       <color theme="1"/>
       <name val="Menlo"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color indexed="14"/>
+      <name val="Menlo"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -361,7 +410,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -498,11 +547,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -537,6 +601,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -819,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -957,7 +1027,7 @@
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="31.2">
       <c r="A7" s="13" t="s">
         <v>61</v>
       </c>
@@ -965,7 +1035,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>39</v>
@@ -1275,6 +1345,112 @@
       </c>
       <c r="H21" s="7" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="46.8">
+      <c r="A22" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" ht="31.2">
+      <c r="A23" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1293,7 +1469,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="31.2">
       <c r="A1" s="5" t="s">
         <v>32</v>
       </c>
@@ -1317,7 +1493,7 @@
       </c>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="31.2">
       <c r="A2" s="5" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Added more controlled weight times for option values and refactored code
</commit_message>
<xml_diff>
--- a/src/test/java/com/seopa/tests/automated/test/cases/CarRegistrationLookUp01.xlsx
+++ b/src/test/java/com/seopa/tests/automated/test/cases/CarRegistrationLookUp01.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patrick.mcparland\Documents\selenium_tests\src\test\java\com\seopa\tests\automated\test\cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickmcparland/java/selenium_tests/src/test/java/com/seopa/tests/automated/test/cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="636" yWindow="1176" windowWidth="28164" windowHeight="16884" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="70">
   <si>
     <t>Element Type</t>
   </si>
@@ -271,9 +271,6 @@
     <t>AUDI</t>
   </si>
   <si>
-    <t>A4</t>
-  </si>
-  <si>
     <t>2013</t>
   </si>
   <si>
@@ -302,9 +299,6 @@
   </si>
   <si>
     <t>//input[@name="vehicle_side" and @value="Y"]</t>
-  </si>
-  <si>
-    <t>fake_vehicle_confirm</t>
   </si>
   <si>
     <r>
@@ -351,7 +345,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -892,16 +886,16 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.296875" style="6" customWidth="1"/>
-    <col min="2" max="8" width="20.296875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" style="6" customWidth="1"/>
+    <col min="2" max="8" width="20.33203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.4">
+    <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>38</v>
       </c>
@@ -927,7 +921,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="46.8">
+    <row r="2" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>50</v>
       </c>
@@ -935,7 +929,7 @@
         <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -947,15 +941,15 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>37</v>
@@ -967,75 +961,75 @@
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="1:8" ht="31.2">
+    <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>37</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:8" ht="31.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>39</v>
@@ -1047,15 +1041,15 @@
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
     </row>
-    <row r="8" spans="1:8" ht="46.8">
+    <row r="8" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>6</v>
@@ -1067,7 +1061,7 @@
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -1089,7 +1083,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1111,7 +1105,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>26</v>
       </c>
@@ -1133,7 +1127,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>15</v>
       </c>
@@ -1155,7 +1149,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
@@ -1175,7 +1169,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" ht="46.8">
+    <row r="14" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -1195,7 +1189,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:8" ht="46.8">
+    <row r="15" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -1215,7 +1209,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" ht="46.8">
+    <row r="16" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>21</v>
       </c>
@@ -1235,7 +1229,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" ht="31.2">
+    <row r="17" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>22</v>
       </c>
@@ -1255,7 +1249,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" ht="62.4">
+    <row r="18" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>24</v>
       </c>
@@ -1275,7 +1269,7 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>25</v>
       </c>
@@ -1295,7 +1289,7 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>32</v>
       </c>
@@ -1321,7 +1315,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>45</v>
       </c>
@@ -1347,7 +1341,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="46.8">
+    <row r="22" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>50</v>
       </c>
@@ -1355,7 +1349,7 @@
         <v>19</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>6</v>
@@ -1367,35 +1361,35 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" ht="31.2">
+    <row r="23" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>6</v>
@@ -1407,27 +1401,27 @@
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>39</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>32</v>
       </c>
@@ -1467,9 +1461,9 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="31.2">
+    <row r="1" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>32</v>
       </c>
@@ -1493,7 +1487,7 @@
       </c>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="31.2">
+    <row r="2" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>45</v>
       </c>

</xml_diff>